<commit_message>
fixed"rxjava" and "kotlin coroutines" issue
added "rxjava" and "kotlin coroutines" to Android specific stack.
</commit_message>
<xml_diff>
--- a/data/all_tables.xlsx
+++ b/data/all_tables.xlsx
@@ -7176,7 +7176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M156"/>
+  <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7804,7 +7804,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>CocoaPods</t>
+          <t>Model-View-Controller (MVC)</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Model-View-Controller (MVC)</t>
+          <t>CocoaPods</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -8275,7 +8275,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Jira</t>
+          <t>Model-View-Presenter (MVP)</t>
         </is>
       </c>
       <c r="L24" t="n">
@@ -8310,7 +8310,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>XCTest</t>
+          <t>Firebase</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -8321,7 +8321,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Model-View-Presenter (MVP)</t>
+          <t>Jira</t>
         </is>
       </c>
       <c r="L25" t="n">
@@ -8356,7 +8356,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Firebase</t>
+          <t>XCTest</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -8505,7 +8505,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>React Native</t>
+          <t>CocoaPods</t>
         </is>
       </c>
       <c r="L29" t="n">
@@ -8551,7 +8551,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>CocoaPods</t>
+          <t>React Native</t>
         </is>
       </c>
       <c r="L30" t="n">
@@ -8781,7 +8781,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Alamofire</t>
+          <t>Facebook SDK</t>
         </is>
       </c>
       <c r="L35" t="n">
@@ -8827,7 +8827,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Facebook SDK</t>
+          <t>Alamofire</t>
         </is>
       </c>
       <c r="L36" t="n">
@@ -8873,7 +8873,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>fastlane</t>
+          <t>GitHub</t>
         </is>
       </c>
       <c r="L37" t="n">
@@ -8908,7 +8908,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>C++</t>
+          <t>Kanban</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -8919,7 +8919,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>SQLite</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="L38" t="n">
@@ -8965,7 +8965,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>SQLite</t>
         </is>
       </c>
       <c r="L39" t="n">
@@ -9046,7 +9046,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Kanban</t>
+          <t>C++</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -9103,7 +9103,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>fastlane</t>
         </is>
       </c>
       <c r="L42" t="n">
@@ -9184,7 +9184,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Human Interface Guidelines</t>
+          <t>GitLab</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -9195,7 +9195,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Flutter</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="L44" t="n">
@@ -9230,7 +9230,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>GitLab</t>
+          <t>Human Interface Guidelines</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -9287,7 +9287,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Flutter</t>
         </is>
       </c>
       <c r="L46" t="n">
@@ -9379,7 +9379,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>SQL</t>
+          <t>Confluence</t>
         </is>
       </c>
       <c r="L48" t="n">
@@ -9425,7 +9425,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Confluence</t>
+          <t>SQL</t>
         </is>
       </c>
       <c r="L49" t="n">
@@ -9460,7 +9460,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Bitrise</t>
+          <t>Alamofire</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -9471,7 +9471,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Figma</t>
+          <t>Swift Package Manager</t>
         </is>
       </c>
       <c r="L50" t="n">
@@ -9506,7 +9506,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Alamofire</t>
+          <t>Bitrise</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -9517,7 +9517,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Swift Package Manager</t>
+          <t>Ionic</t>
         </is>
       </c>
       <c r="L51" t="n">
@@ -9552,7 +9552,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>WebSockets</t>
+          <t>Amazon Web Services (AWS)</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Realm</t>
+          <t>Bluetooth</t>
         </is>
       </c>
       <c r="L52" t="n">
@@ -9598,7 +9598,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Amazon Web Services (AWS)</t>
+          <t>WebSockets</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -9609,7 +9609,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Bluetooth</t>
+          <t>Realm</t>
         </is>
       </c>
       <c r="L53" t="n">
@@ -9644,7 +9644,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Kotlin Multiplatform</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -9655,7 +9655,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Ionic</t>
+          <t>Figma</t>
         </is>
       </c>
       <c r="L54" t="n">
@@ -9690,7 +9690,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Kotlin Multiplatform</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -9701,7 +9701,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Apache Cordova</t>
+          <t>Keychain</t>
         </is>
       </c>
       <c r="L55" t="n">
@@ -9736,7 +9736,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>Crashlytics</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -9782,7 +9782,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Crashlytics</t>
+          <t>GitHub</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -9793,7 +9793,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>Keychain</t>
+          <t>Apache Cordova</t>
         </is>
       </c>
       <c r="L57" t="n">
@@ -9874,7 +9874,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Core Location</t>
+          <t>TypeScript</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -9885,7 +9885,7 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>Amazon Web Services (AWS)</t>
+          <t>MongoDB</t>
         </is>
       </c>
       <c r="L59" t="n">
@@ -9920,7 +9920,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>GitHub Actions</t>
+          <t>Bluetooth</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -9966,7 +9966,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>TypeScript</t>
+          <t>Core Location</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -9977,7 +9977,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>MongoDB</t>
+          <t>Amazon Web Services (AWS)</t>
         </is>
       </c>
       <c r="L61" t="n">
@@ -10012,7 +10012,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Bluetooth</t>
+          <t>GitHub Actions</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -10023,7 +10023,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Docker</t>
+          <t>Xamarin</t>
         </is>
       </c>
       <c r="L62" t="n">
@@ -10069,7 +10069,7 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>OAuth</t>
+          <t>AVPlayer</t>
         </is>
       </c>
       <c r="L63" t="n">
@@ -10104,7 +10104,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>ARKit</t>
+          <t>Xamarin</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>AVPlayer</t>
+          <t>OAuth</t>
         </is>
       </c>
       <c r="L64" t="n">
@@ -10150,7 +10150,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Figma</t>
+          <t>ARKit</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -10161,7 +10161,7 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>Bazel</t>
+          <t>Docker</t>
         </is>
       </c>
       <c r="L65" t="n">
@@ -10196,7 +10196,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Xamarin</t>
+          <t>Figma</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -10207,7 +10207,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>WebKit</t>
+          <t>TestFlight</t>
         </is>
       </c>
       <c r="L66" t="n">
@@ -10253,7 +10253,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Grand Central Dispatch (GCD)</t>
+          <t>CircleCI</t>
         </is>
       </c>
       <c r="L67" t="n">
@@ -10288,7 +10288,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>MapKit</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -10299,7 +10299,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Xamarin</t>
+          <t>Grand Central Dispatch (GCD)</t>
         </is>
       </c>
       <c r="L68" t="n">
@@ -10334,7 +10334,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>MapKit</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -10345,7 +10345,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Core Location</t>
+          <t>Go</t>
         </is>
       </c>
       <c r="L69" t="n">
@@ -10380,7 +10380,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Carthage</t>
+          <t>C#</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -10391,7 +10391,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>CircleCI</t>
+          <t>GitLab</t>
         </is>
       </c>
       <c r="L70" t="n">
@@ -10426,7 +10426,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>C#</t>
+          <t>URLSession</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -10437,7 +10437,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>TestFlight</t>
+          <t>WebKit</t>
         </is>
       </c>
       <c r="L71" t="n">
@@ -10472,7 +10472,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>URLSession</t>
+          <t>Carthage</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -10483,7 +10483,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>GitLab</t>
+          <t>Core Location</t>
         </is>
       </c>
       <c r="L72" t="n">
@@ -10518,7 +10518,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>PHP</t>
+          <t>Apache Cordova</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -10529,7 +10529,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Go</t>
+          <t>Bazel</t>
         </is>
       </c>
       <c r="L73" t="n">
@@ -10564,7 +10564,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Redux</t>
+          <t>Docker</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -10610,7 +10610,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>SQL</t>
+          <t>View-Interactor-Presenter (VIP)</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -10621,7 +10621,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Swinject</t>
+          <t>Bitrise</t>
         </is>
       </c>
       <c r="L75" t="n">
@@ -10656,7 +10656,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>TeamCity</t>
+          <t>Redux</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -10667,7 +10667,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Bitrise</t>
+          <t>Bitbucket</t>
         </is>
       </c>
       <c r="L76" t="n">
@@ -10702,7 +10702,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Unity Engine</t>
+          <t>Keychain</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -10713,7 +10713,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Bitbucket</t>
+          <t>XCUITest</t>
         </is>
       </c>
       <c r="L77" t="n">
@@ -10748,7 +10748,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>View-Interactor-Presenter (VIP)</t>
+          <t>Zeplin</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -10759,7 +10759,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>XCUITest</t>
+          <t>Swinject</t>
         </is>
       </c>
       <c r="L78" t="n">
@@ -10794,7 +10794,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>XCUITest</t>
+          <t>Unity Engine</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -10840,7 +10840,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Zeplin</t>
+          <t>XCUITest</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -10851,7 +10851,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>WebSockets</t>
+          <t>TypeScript</t>
         </is>
       </c>
       <c r="L80" t="n">
@@ -10886,7 +10886,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Keychain</t>
+          <t>TeamCity</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -10932,7 +10932,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Apache Cordova</t>
+          <t>PHP</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -10943,7 +10943,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Stripe SDK</t>
+          <t>Redux</t>
         </is>
       </c>
       <c r="L82" t="n">
@@ -10978,7 +10978,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Docker</t>
+          <t>SQL</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -11024,7 +11024,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>MySQL</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -11035,7 +11035,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Visual Basic</t>
+          <t>Stripe SDK</t>
         </is>
       </c>
       <c r="L84" t="n">
@@ -11070,7 +11070,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Go</t>
+          <t>CircleCI</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -11081,7 +11081,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Redux</t>
+          <t>Visual Basic</t>
         </is>
       </c>
       <c r="L85" t="n">
@@ -11116,7 +11116,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Bamboo</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -11127,7 +11127,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>TypeScript</t>
+          <t>Waterfall</t>
         </is>
       </c>
       <c r="L86" t="n">
@@ -11162,7 +11162,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Behavior-Driven Development (BDD)</t>
+          <t>AVFoundation</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -11173,7 +11173,7 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Waterfall</t>
+          <t>WebSockets</t>
         </is>
       </c>
       <c r="L87" t="n">
@@ -11208,7 +11208,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>CircleCI</t>
+          <t>Behavior-Driven Development (BDD)</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -11254,7 +11254,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Google Analytics</t>
+          <t>Bamboo</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -11300,7 +11300,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Gradle</t>
+          <t>Go</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>Apache Maven</t>
+          <t>Dart</t>
         </is>
       </c>
       <c r="L90" t="n">
@@ -11346,7 +11346,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>AVFoundation</t>
+          <t>Google Analytics</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -11357,7 +11357,7 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>GitFlow</t>
+          <t>AWS Lambda</t>
         </is>
       </c>
       <c r="L91" t="n">
@@ -11392,7 +11392,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>MySQL</t>
+          <t>Gradle</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -11403,7 +11403,7 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>Google Cloud Messaging</t>
+          <t>Microsoft SQL Server</t>
         </is>
       </c>
       <c r="L92" t="n">
@@ -11438,7 +11438,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>OAuth 2.0</t>
+          <t>Ruby</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -11449,7 +11449,7 @@
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>Google Maps</t>
+          <t>Microsoft Azure</t>
         </is>
       </c>
       <c r="L93" t="n">
@@ -11484,7 +11484,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Sentry</t>
+          <t>Camera</t>
         </is>
       </c>
       <c r="I94" t="n">
@@ -11495,7 +11495,7 @@
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>Camera</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="L94" t="n">
@@ -11530,7 +11530,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Ruby</t>
+          <t>Core Bluetooth</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -11541,7 +11541,7 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>HealthKit</t>
+          <t>GitFlow</t>
         </is>
       </c>
       <c r="L95" t="n">
@@ -11576,7 +11576,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Core Bluetooth</t>
+          <t>Sentry</t>
         </is>
       </c>
       <c r="I96" t="n">
@@ -11587,7 +11587,7 @@
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>Behavior-Driven Development (BDD)</t>
+          <t>Apache Maven</t>
         </is>
       </c>
       <c r="L96" t="n">
@@ -11622,7 +11622,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Camera</t>
+          <t>OAuth</t>
         </is>
       </c>
       <c r="I97" t="n">
@@ -11633,7 +11633,7 @@
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>Dart</t>
+          <t>Google Cloud Messaging</t>
         </is>
       </c>
       <c r="L97" t="n">
@@ -11668,7 +11668,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>OAuth</t>
+          <t>watchOS</t>
         </is>
       </c>
       <c r="I98" t="n">
@@ -11679,7 +11679,7 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Google Maps</t>
         </is>
       </c>
       <c r="L98" t="n">
@@ -11714,7 +11714,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>watchOS</t>
+          <t>OAuth 2.0</t>
         </is>
       </c>
       <c r="I99" t="n">
@@ -11725,7 +11725,7 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Microsoft Azure</t>
+          <t>Behavior-Driven Development (BDD)</t>
         </is>
       </c>
       <c r="L99" t="n">
@@ -11771,7 +11771,7 @@
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>Microsoft SQL Server</t>
+          <t>HealthKit</t>
         </is>
       </c>
       <c r="L100" t="n">
@@ -11817,7 +11817,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>AWS Lambda</t>
+          <t>Camera</t>
         </is>
       </c>
       <c r="L101" t="n">
@@ -11852,7 +11852,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Node.js</t>
+          <t>Scaled Agile Framework (SAFe)</t>
         </is>
       </c>
       <c r="I102" t="n">
@@ -11863,7 +11863,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>Amplitude</t>
+          <t>WatchKit</t>
         </is>
       </c>
       <c r="L102" t="n">
@@ -11898,7 +11898,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Cloud Firestore</t>
+          <t>Sensors</t>
         </is>
       </c>
       <c r="I103" t="n">
@@ -11909,7 +11909,7 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>Appium</t>
+          <t>URLSession</t>
         </is>
       </c>
       <c r="L103" t="n">
@@ -11944,7 +11944,7 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Stripe SDK</t>
+          <t>Xcode Cloud</t>
         </is>
       </c>
       <c r="I104" t="n">
@@ -11955,7 +11955,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>Crashlytics</t>
+          <t>CarPlay</t>
         </is>
       </c>
       <c r="L104" t="n">
@@ -11990,7 +11990,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Core Motion</t>
+          <t>SonarQube</t>
         </is>
       </c>
       <c r="I105" t="n">
@@ -12001,7 +12001,7 @@
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>Advanced Encryption Standard (AES)</t>
+          <t>Bamboo</t>
         </is>
       </c>
       <c r="L105" t="n">
@@ -12036,7 +12036,7 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>NoSQL</t>
+          <t>Stripe SDK</t>
         </is>
       </c>
       <c r="I106" t="n">
@@ -12082,7 +12082,7 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>SwiftLint</t>
+          <t>Swift Concurrency</t>
         </is>
       </c>
       <c r="I107" t="n">
@@ -12093,7 +12093,7 @@
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>WatchKit</t>
+          <t>Crashlytics</t>
         </is>
       </c>
       <c r="L107" t="n">
@@ -12128,7 +12128,7 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>Core Audio</t>
+          <t>NoSQL</t>
         </is>
       </c>
       <c r="I108" t="n">
@@ -12139,7 +12139,7 @@
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>CarPlay</t>
+          <t>Appium</t>
         </is>
       </c>
       <c r="L108" t="n">
@@ -12174,7 +12174,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>Swinject</t>
+          <t>gRPC</t>
         </is>
       </c>
       <c r="I109" t="n">
@@ -12185,7 +12185,7 @@
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>Zeplin</t>
+          <t>Amplitude</t>
         </is>
       </c>
       <c r="L109" t="n">
@@ -12220,7 +12220,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Mixpanel</t>
+          <t>SwiftLint</t>
         </is>
       </c>
       <c r="I110" t="n">
@@ -12231,7 +12231,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>AWS Amplify</t>
+          <t>Advanced Encryption Standard (AES)</t>
         </is>
       </c>
       <c r="L110" t="n">
@@ -12266,7 +12266,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Sensors</t>
+          <t>Appium</t>
         </is>
       </c>
       <c r="I111" t="n">
@@ -12277,7 +12277,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>URLSession</t>
+          <t>Zeplin</t>
         </is>
       </c>
       <c r="L111" t="n">
@@ -12312,7 +12312,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Microsoft Azure</t>
+          <t>Swinject</t>
         </is>
       </c>
       <c r="I112" t="n">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>Core ML</t>
+          <t>AWS Amplify</t>
         </is>
       </c>
       <c r="L112" t="n">
@@ -12358,7 +12358,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Unity Cloud Build</t>
+          <t>Gerrit</t>
         </is>
       </c>
       <c r="I113" t="n">
@@ -12369,7 +12369,7 @@
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>Bamboo</t>
+          <t>Core ML</t>
         </is>
       </c>
       <c r="L113" t="n">
@@ -12404,7 +12404,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Metal</t>
+          <t>AVKit</t>
         </is>
       </c>
       <c r="I114" t="n">
@@ -12415,7 +12415,7 @@
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>NFC</t>
+          <t>Parse Platform</t>
         </is>
       </c>
       <c r="L114" t="n">
@@ -12450,7 +12450,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Appium</t>
+          <t>Unity Cloud Build</t>
         </is>
       </c>
       <c r="I115" t="n">
@@ -12496,7 +12496,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Xcode Cloud</t>
+          <t>Node.js</t>
         </is>
       </c>
       <c r="I116" t="n">
@@ -12507,7 +12507,7 @@
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>TLS Pinning</t>
+          <t>Rust</t>
         </is>
       </c>
       <c r="L116" t="n">
@@ -12542,7 +12542,7 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>gRPC</t>
+          <t>Microsoft Azure</t>
         </is>
       </c>
       <c r="I117" t="n">
@@ -12553,7 +12553,7 @@
       </c>
       <c r="K117" t="inlineStr">
         <is>
-          <t>PayPal SDK</t>
+          <t>NFC</t>
         </is>
       </c>
       <c r="L117" t="n">
@@ -12588,7 +12588,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>AVKit</t>
+          <t>Core Motion</t>
         </is>
       </c>
       <c r="I118" t="n">
@@ -12634,7 +12634,7 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>SonarQube</t>
+          <t>Core Audio</t>
         </is>
       </c>
       <c r="I119" t="n">
@@ -12680,7 +12680,7 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Swift Concurrency</t>
+          <t>Open Web Application Security Project (OWASP)</t>
         </is>
       </c>
       <c r="I120" t="n">
@@ -12691,7 +12691,7 @@
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>MapKit</t>
+          <t>Retrofit</t>
         </is>
       </c>
       <c r="L120" t="n">
@@ -12726,7 +12726,7 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Dart</t>
+          <t>Moya</t>
         </is>
       </c>
       <c r="I121" t="n">
@@ -12737,7 +12737,7 @@
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>Retrofit</t>
+          <t>Rivest–Shamir–Adleman (RSA)</t>
         </is>
       </c>
       <c r="L121" t="n">
@@ -12772,7 +12772,7 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Gerrit</t>
+          <t>Protocol Buffers</t>
         </is>
       </c>
       <c r="I122" t="n">
@@ -12783,7 +12783,7 @@
       </c>
       <c r="K122" t="inlineStr">
         <is>
-          <t>Rivest–Shamir–Adleman (RSA)</t>
+          <t>Ruby</t>
         </is>
       </c>
       <c r="L122" t="n">
@@ -12818,7 +12818,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Scaled Agile Framework (SAFe)</t>
+          <t>Cloud Firestore</t>
         </is>
       </c>
       <c r="I123" t="n">
@@ -12829,7 +12829,7 @@
       </c>
       <c r="K123" t="inlineStr">
         <is>
-          <t>Ruby</t>
+          <t>MapKit</t>
         </is>
       </c>
       <c r="L123" t="n">
@@ -12864,7 +12864,7 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Protocol Buffers</t>
+          <t>Model-View-Intent (MVI)</t>
         </is>
       </c>
       <c r="I124" t="n">
@@ -12875,7 +12875,7 @@
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>Rust</t>
+          <t>TLS Pinning</t>
         </is>
       </c>
       <c r="L124" t="n">
@@ -12910,7 +12910,7 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Moya</t>
+          <t>Dart</t>
         </is>
       </c>
       <c r="I125" t="n">
@@ -12956,7 +12956,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Open Web Application Security Project (OWASP)</t>
+          <t>Mixpanel</t>
         </is>
       </c>
       <c r="I126" t="n">
@@ -12967,7 +12967,7 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>Kotlin Coroutines</t>
+          <t>JUnit</t>
         </is>
       </c>
       <c r="L126" t="n">
@@ -13002,7 +13002,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Model-View-Intent (MVI)</t>
+          <t>Metal</t>
         </is>
       </c>
       <c r="I127" t="n">
@@ -13013,7 +13013,7 @@
       </c>
       <c r="K127" t="inlineStr">
         <is>
-          <t>JUnit</t>
+          <t>Sensors</t>
         </is>
       </c>
       <c r="L127" t="n">
@@ -13059,7 +13059,7 @@
       </c>
       <c r="K128" t="inlineStr">
         <is>
-          <t>Sensors</t>
+          <t>SonarQube</t>
         </is>
       </c>
       <c r="L128" t="n">
@@ -13105,7 +13105,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>SonarQube</t>
+          <t>HTML</t>
         </is>
       </c>
       <c r="L129" t="n">
@@ -13132,7 +13132,7 @@
       <c r="F130" t="inlineStr"/>
       <c r="H130" t="inlineStr">
         <is>
-          <t>OpenAPI</t>
+          <t>App Center</t>
         </is>
       </c>
       <c r="I130" t="n">
@@ -13143,7 +13143,7 @@
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>HTML</t>
+          <t>PayPal SDK</t>
         </is>
       </c>
       <c r="L130" t="n">
@@ -13170,7 +13170,7 @@
       <c r="F131" t="inlineStr"/>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Amazon S3</t>
+          <t>Apache Maven</t>
         </is>
       </c>
       <c r="I131" t="n">
@@ -13181,7 +13181,7 @@
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>Parse Platform</t>
+          <t>Frida</t>
         </is>
       </c>
       <c r="L131" t="n">
@@ -13217,17 +13217,9 @@
       <c r="J132" t="n">
         <v>0.13</v>
       </c>
-      <c r="K132" t="inlineStr">
-        <is>
-          <t>Frida</t>
-        </is>
-      </c>
-      <c r="L132" t="n">
-        <v>1</v>
-      </c>
-      <c r="M132" t="n">
-        <v>0.37</v>
-      </c>
+      <c r="K132" t="inlineStr"/>
+      <c r="L132" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -13246,7 +13238,7 @@
       <c r="F133" t="inlineStr"/>
       <c r="H133" t="inlineStr">
         <is>
-          <t>NFC</t>
+          <t>Amazon S3</t>
         </is>
       </c>
       <c r="I133" t="n">
@@ -13276,7 +13268,7 @@
       <c r="F134" t="inlineStr"/>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Apache Maven</t>
+          <t>Azure DevOps</t>
         </is>
       </c>
       <c r="I134" t="n">
@@ -13306,7 +13298,7 @@
       <c r="F135" t="inlineStr"/>
       <c r="H135" t="inlineStr">
         <is>
-          <t>App Center</t>
+          <t>Trello</t>
         </is>
       </c>
       <c r="I135" t="n">
@@ -13336,7 +13328,7 @@
       <c r="F136" t="inlineStr"/>
       <c r="H136" t="inlineStr">
         <is>
-          <t>PayPal SDK</t>
+          <t>Google Cloud Platform</t>
         </is>
       </c>
       <c r="I136" t="n">
@@ -13366,7 +13358,7 @@
       <c r="F137" t="inlineStr"/>
       <c r="H137" t="inlineStr">
         <is>
-          <t>Azure DevOps</t>
+          <t>TLS Pinning</t>
         </is>
       </c>
       <c r="I137" t="n">
@@ -13396,7 +13388,7 @@
       <c r="F138" t="inlineStr"/>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Bazel</t>
+          <t>Cydia Substrate</t>
         </is>
       </c>
       <c r="I138" t="n">
@@ -13412,7 +13404,7 @@
     <row r="139">
       <c r="H139" t="inlineStr">
         <is>
-          <t>Google Maps</t>
+          <t>HTML</t>
         </is>
       </c>
       <c r="I139" t="n">
@@ -13428,7 +13420,7 @@
     <row r="140">
       <c r="H140" t="inlineStr">
         <is>
-          <t>Google Cloud Platform</t>
+          <t>Frida</t>
         </is>
       </c>
       <c r="I140" t="n">
@@ -13444,7 +13436,7 @@
     <row r="141">
       <c r="H141" t="inlineStr">
         <is>
-          <t>Cydia Substrate</t>
+          <t>JUnit</t>
         </is>
       </c>
       <c r="I141" t="n">
@@ -13460,7 +13452,7 @@
     <row r="142">
       <c r="H142" t="inlineStr">
         <is>
-          <t>Microsoft SQL Server</t>
+          <t>Facebook SDK</t>
         </is>
       </c>
       <c r="I142" t="n">
@@ -13476,7 +13468,7 @@
     <row r="143">
       <c r="H143" t="inlineStr">
         <is>
-          <t>Trello</t>
+          <t>Datadog</t>
         </is>
       </c>
       <c r="I143" t="n">
@@ -13492,7 +13484,7 @@
     <row r="144">
       <c r="H144" t="inlineStr">
         <is>
-          <t>CarPlay</t>
+          <t>Microsoft SQL Server</t>
         </is>
       </c>
       <c r="I144" t="n">
@@ -13508,7 +13500,7 @@
     <row r="145">
       <c r="H145" t="inlineStr">
         <is>
-          <t>Frida</t>
+          <t>Mockito</t>
         </is>
       </c>
       <c r="I145" t="n">
@@ -13524,7 +13516,7 @@
     <row r="146">
       <c r="H146" t="inlineStr">
         <is>
-          <t>TLS Pinning</t>
+          <t>NFC</t>
         </is>
       </c>
       <c r="I146" t="n">
@@ -13540,7 +13532,7 @@
     <row r="147">
       <c r="H147" t="inlineStr">
         <is>
-          <t>Facebook SDK</t>
+          <t>Bazel</t>
         </is>
       </c>
       <c r="I147" t="n">
@@ -13556,7 +13548,7 @@
     <row r="148">
       <c r="H148" t="inlineStr">
         <is>
-          <t>Rivest–Shamir–Adleman (RSA)</t>
+          <t>OpenAPI</t>
         </is>
       </c>
       <c r="I148" t="n">
@@ -13572,7 +13564,7 @@
     <row r="149">
       <c r="H149" t="inlineStr">
         <is>
-          <t>Room</t>
+          <t>PayPal SDK</t>
         </is>
       </c>
       <c r="I149" t="n">
@@ -13588,7 +13580,7 @@
     <row r="150">
       <c r="H150" t="inlineStr">
         <is>
-          <t>Mockito</t>
+          <t>Google Maps</t>
         </is>
       </c>
       <c r="I150" t="n">
@@ -13604,7 +13596,7 @@
     <row r="151">
       <c r="H151" t="inlineStr">
         <is>
-          <t>HTML</t>
+          <t>Rivest–Shamir–Adleman (RSA)</t>
         </is>
       </c>
       <c r="I151" t="n">
@@ -13620,7 +13612,7 @@
     <row r="152">
       <c r="H152" t="inlineStr">
         <is>
-          <t>RxJava</t>
+          <t>Room</t>
         </is>
       </c>
       <c r="I152" t="n">
@@ -13636,7 +13628,7 @@
     <row r="153">
       <c r="H153" t="inlineStr">
         <is>
-          <t>Swagger</t>
+          <t>CSS</t>
         </is>
       </c>
       <c r="I153" t="n">
@@ -13652,7 +13644,7 @@
     <row r="154">
       <c r="H154" t="inlineStr">
         <is>
-          <t>Datadog</t>
+          <t>Swagger</t>
         </is>
       </c>
       <c r="I154" t="n">
@@ -13668,7 +13660,7 @@
     <row r="155">
       <c r="H155" t="inlineStr">
         <is>
-          <t>JUnit</t>
+          <t>CarPlay</t>
         </is>
       </c>
       <c r="I155" t="n">
@@ -13680,22 +13672,6 @@
       <c r="K155" t="inlineStr"/>
       <c r="L155" t="inlineStr"/>
       <c r="M155" t="inlineStr"/>
-    </row>
-    <row r="156">
-      <c r="H156" t="inlineStr">
-        <is>
-          <t>CSS</t>
-        </is>
-      </c>
-      <c r="I156" t="n">
-        <v>1</v>
-      </c>
-      <c r="J156" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="K156" t="inlineStr"/>
-      <c r="L156" t="inlineStr"/>
-      <c r="M156" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -15426,7 +15402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15687,33 +15663,9 @@
       <c r="J6" t="n">
         <v>0.27</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Kotlin Coroutines</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>RxJava</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
fixed "hig" in Android stack
</commit_message>
<xml_diff>
--- a/data/all_tables.xlsx
+++ b/data/all_tables.xlsx
@@ -1538,7 +1538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1672,22 +1672,6 @@
       <c r="M3" t="n">
         <v>3.69</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Human Interface Guidelines</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9070,7 +9054,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mockito</t>
+          <t>Docker</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -9116,7 +9100,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Java Native Interface (JNI)</t>
+          <t>Notifications</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -9162,7 +9146,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Docker</t>
+          <t>Java Native Interface (JNI)</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -9208,7 +9192,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Notifications</t>
+          <t>Mockito</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -9438,7 +9422,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>React Native</t>
+          <t>fastlane</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -9484,7 +9468,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>fastlane</t>
+          <t>React Native</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -9622,7 +9606,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Android Compatibility Test Suite (CTS)</t>
+          <t>Gerrit</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -9668,7 +9652,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Gerrit</t>
+          <t>Android Compatibility Test Suite (CTS)</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -9806,7 +9790,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Crashlytics</t>
+          <t>OkHttp</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -9852,7 +9836,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>OkHttp</t>
+          <t>Crashlytics</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -9898,7 +9882,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SonarQube</t>
+          <t>Bluetooth Low Energy (BLE)</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -9990,7 +9974,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Bluetooth Low Energy (BLE)</t>
+          <t>SonarQube</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -10128,7 +10112,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Binder</t>
+          <t>C#</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -10174,7 +10158,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>C#</t>
+          <t>Binder</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -10220,7 +10204,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Android Auto</t>
+          <t>Amazon Web Services (AWS)</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -10266,7 +10250,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Amazon Web Services (AWS)</t>
+          <t>Figma</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -10312,7 +10296,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Figma</t>
+          <t>Android Auto</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -10450,7 +10434,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>TypeScript</t>
+          <t>Bamboo</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -10496,7 +10480,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Bamboo</t>
+          <t>Behavior-Driven Development (BDD)</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -10542,7 +10526,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Bitbucket</t>
+          <t>Glide</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -10588,7 +10572,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Glide</t>
+          <t>TypeScript</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -10634,7 +10618,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Behavior-Driven Development (BDD)</t>
+          <t>Bitbucket</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -10680,7 +10664,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Apache Maven</t>
+          <t>NoSQL</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -10726,7 +10710,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Robolectric</t>
+          <t>Apache Maven</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -10772,7 +10756,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>NoSQL</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -10818,7 +10802,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Sensors</t>
+          <t>Robolectric</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -10864,7 +10848,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Sensors</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -10910,7 +10894,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Node.js</t>
+          <t>Go</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -10956,7 +10940,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Go</t>
+          <t>Apache Cordova</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -11002,7 +10986,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>ExoPlayer</t>
+          <t>Node.js</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -11048,7 +11032,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Dart</t>
+          <t>ExoPlayer</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -11094,7 +11078,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>CircleCI</t>
+          <t>Android Open Source Project (AOSP)</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -11140,7 +11124,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Bluetooth</t>
+          <t>Swagger</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -11186,7 +11170,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Swagger</t>
+          <t>Android TV</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -11232,7 +11216,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Apache Cordova</t>
+          <t>Dart</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -11278,7 +11262,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Android TV</t>
+          <t>CircleCI</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -11324,7 +11308,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Android Open Source Project (AOSP)</t>
+          <t>Bluetooth</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -11370,7 +11354,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Rust</t>
+          <t>WebSockets</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -11416,7 +11400,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>RxKotlin</t>
+          <t>WebView</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -11462,7 +11446,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>WebSockets</t>
+          <t>Xamarin</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -11508,7 +11492,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>WebView</t>
+          <t>RxKotlin</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -11554,7 +11538,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Xamarin</t>
+          <t>Rust</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -12290,7 +12274,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Apache Groovy</t>
+          <t>Ionic</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -12336,7 +12320,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Ionic</t>
+          <t>Android Profiler</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -12428,7 +12412,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Human Interface Guidelines</t>
+          <t>Redux</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -12474,7 +12458,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Redux</t>
+          <t>Microsoft Azure</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -12520,7 +12504,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Microsoft Azure</t>
+          <t>Protocol Buffers</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -12566,7 +12550,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Protocol Buffers</t>
+          <t>PHP</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -12612,7 +12596,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>PHP</t>
+          <t>OpenAPI</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -12658,7 +12642,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>OpenAPI</t>
+          <t>Apache Groovy</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -12704,14 +12688,14 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Android Profiler</t>
+          <t>App Center</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C121" t="n">
-        <v>0.29</v>
+        <v>0.15</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -12750,7 +12734,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>App Center</t>
+          <t>Trello</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -12796,7 +12780,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Trello</t>
+          <t>Amplitude</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -12842,7 +12826,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Amplitude</t>
+          <t>Yocto Project</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -12888,7 +12872,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Yocto Project</t>
+          <t>Amazon S3</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -12934,7 +12918,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Amazon S3</t>
+          <t>Appium</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -12980,7 +12964,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Appium</t>
+          <t>OAuth 2.0</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -13026,7 +13010,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>OAuth</t>
+          <t>Spring Boot</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -13072,7 +13056,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Spring Boot</t>
+          <t>OAuth</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -13118,7 +13102,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>OAuth 2.0</t>
+          <t>General Data Protection Regulation (GDPR)</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -13156,7 +13140,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>General Data Protection Regulation (GDPR)</t>
+          <t>Ghidra</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -13194,7 +13178,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Ghidra</t>
+          <t>Ruby</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -13224,7 +13208,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Ruby</t>
+          <t>Google Cloud Messaging</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -13254,7 +13238,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Google Cloud Messaging</t>
+          <t>MongoDB</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -13284,7 +13268,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>MongoDB</t>
+          <t>NFC</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -13344,7 +13328,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>NFC</t>
+          <t>Facebook SDK</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -13372,20 +13356,6 @@
       <c r="M137" t="inlineStr"/>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>Facebook SDK</t>
-        </is>
-      </c>
-      <c r="B138" t="n">
-        <v>1</v>
-      </c>
-      <c r="C138" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D138" t="inlineStr"/>
-      <c r="E138" t="inlineStr"/>
-      <c r="F138" t="inlineStr"/>
       <c r="H138" t="inlineStr">
         <is>
           <t>Cydia Substrate</t>

</xml_diff>